<commit_message>
finished with spreadsheet, simulation 5
</commit_message>
<xml_diff>
--- a/Simulation Suites/EM_Simulation_V5/Simulation Summary 8 Iterations.xlsx
+++ b/Simulation Suites/EM_Simulation_V5/Simulation Summary 8 Iterations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jess/git/economic-model/Simulation Suites/EM_Simulation_V5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2F4E36-8BA9-C743-BD7C-C94A9E8E1A3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF6299D-C4D2-024B-A437-406DAD20047A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1740" windowWidth="28040" windowHeight="17440" xr2:uid="{131058AE-3640-E443-9E55-C19E5316A83A}"/>
+    <workbookView xWindow="3940" yWindow="2000" windowWidth="28040" windowHeight="17440" xr2:uid="{131058AE-3640-E443-9E55-C19E5316A83A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
   <si>
     <t>Total</t>
   </si>
@@ -100,13 +100,16 @@
   </si>
   <si>
     <t>Scenario 5</t>
+  </si>
+  <si>
+    <t>Scenario 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +145,14 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -188,6 +199,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DE7D1A-F755-534C-81DC-12F5783227F8}">
-  <dimension ref="B7:O35"/>
+  <dimension ref="B7:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -820,7 +834,7 @@
         <v>0.11084444444444444</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>16</v>
       </c>
@@ -831,7 +845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C19" s="5" t="s">
         <v>11</v>
       </c>
@@ -869,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>1</v>
       </c>
@@ -901,7 +915,7 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>2</v>
       </c>
@@ -933,7 +947,7 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>3</v>
       </c>
@@ -965,7 +979,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>4</v>
       </c>
@@ -1001,7 +1015,7 @@
       </c>
       <c r="L23" s="8">
         <f>ROUND(AVERAGE(F28:F35),0)</f>
-        <v>10178</v>
+        <v>10463</v>
       </c>
       <c r="M23" s="9">
         <f>J23/(I23-K23)</f>
@@ -1009,14 +1023,14 @@
       </c>
       <c r="N23" s="9">
         <f>L23/(I23-K23)</f>
-        <v>0.61812688363053891</v>
+        <v>0.6354354080788297</v>
       </c>
       <c r="O23" s="10">
         <f>N23+M23</f>
-        <v>0.98269147555170921</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>5</v>
       </c>
@@ -1067,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>6</v>
       </c>
@@ -1093,39 +1107,73 @@
       <c r="I25" s="3">
         <v>19760</v>
       </c>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="J25" s="8">
+        <f>AVERAGE(N28:N35)</f>
+        <v>4674.875</v>
+      </c>
+      <c r="K25" s="8">
+        <f>AVERAGE(O28:O35)</f>
+        <v>9379.5</v>
+      </c>
+      <c r="L25" s="8">
+        <f>AVERAGE(P28:P35)</f>
+        <v>5705.625</v>
+      </c>
+      <c r="M25" s="9">
+        <f>J25/(I25-K25)</f>
+        <v>0.45035162082751312</v>
+      </c>
+      <c r="N25" s="9">
+        <f>L25/(I25-K25)</f>
+        <v>0.54964837917248688</v>
+      </c>
+      <c r="O25" s="10">
+        <f>N25+M25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J27" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="K27" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="L27" s="1"/>
+      <c r="M27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="P27" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C28" s="3">
         <v>1</v>
       </c>
@@ -1138,7 +1186,7 @@
       <c r="F28" s="7">
         <v>9649</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <f>F28+E28+D28</f>
         <v>19760</v>
       </c>
@@ -1158,8 +1206,24 @@
         <f>K28+J28+I28</f>
         <v>19760</v>
       </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M28" s="3">
+        <v>1</v>
+      </c>
+      <c r="N28" s="7">
+        <v>4332</v>
+      </c>
+      <c r="O28" s="7">
+        <v>8404</v>
+      </c>
+      <c r="P28" s="7">
+        <v>7024</v>
+      </c>
+      <c r="Q28" s="1">
+        <f>P28+O28+N28</f>
+        <v>19760</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C29" s="3">
         <v>2</v>
       </c>
@@ -1172,7 +1236,7 @@
       <c r="F29" s="7">
         <v>12903</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <f t="shared" ref="G29:G35" si="5">F29+E29+D29</f>
         <v>19760</v>
       </c>
@@ -1192,8 +1256,24 @@
         <f>K29+J29+I29</f>
         <v>19760</v>
       </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M29" s="3">
+        <v>2</v>
+      </c>
+      <c r="N29" s="7">
+        <v>5589</v>
+      </c>
+      <c r="O29" s="7">
+        <v>11145</v>
+      </c>
+      <c r="P29" s="7">
+        <v>3026</v>
+      </c>
+      <c r="Q29" s="1">
+        <f>P29+O29+N29</f>
+        <v>19760</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C30" s="3">
         <v>3</v>
       </c>
@@ -1206,7 +1286,7 @@
       <c r="F30" s="7">
         <v>10730</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <f t="shared" si="5"/>
         <v>19760</v>
       </c>
@@ -1226,8 +1306,24 @@
         <f>K30+J30+I30</f>
         <v>19760</v>
       </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M30" s="3">
+        <v>3</v>
+      </c>
+      <c r="N30" s="7">
+        <v>4440</v>
+      </c>
+      <c r="O30" s="7">
+        <v>8733</v>
+      </c>
+      <c r="P30" s="7">
+        <v>6587</v>
+      </c>
+      <c r="Q30" s="1">
+        <f>P30+O30+N30</f>
+        <v>19760</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C31" s="3">
         <v>4</v>
       </c>
@@ -1240,7 +1336,7 @@
       <c r="F31" s="7">
         <v>11743</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <f t="shared" si="5"/>
         <v>19760</v>
       </c>
@@ -1260,8 +1356,24 @@
         <f>K31+J31+I31</f>
         <v>19760</v>
       </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M31" s="3">
+        <v>4</v>
+      </c>
+      <c r="N31" s="7">
+        <v>3624</v>
+      </c>
+      <c r="O31" s="7">
+        <v>7881</v>
+      </c>
+      <c r="P31" s="7">
+        <v>8255</v>
+      </c>
+      <c r="Q31" s="1">
+        <f>P31+O31+N31</f>
+        <v>19760</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C32" s="3">
         <v>5</v>
       </c>
@@ -1274,7 +1386,7 @@
       <c r="F32" s="7">
         <v>11320</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <f t="shared" si="5"/>
         <v>19760</v>
       </c>
@@ -1294,8 +1406,24 @@
         <f>K32+J32+I32</f>
         <v>19760</v>
       </c>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M32" s="3">
+        <v>5</v>
+      </c>
+      <c r="N32" s="7">
+        <v>4579</v>
+      </c>
+      <c r="O32" s="7">
+        <v>9081</v>
+      </c>
+      <c r="P32" s="7">
+        <v>6100</v>
+      </c>
+      <c r="Q32" s="1">
+        <f>P32+O32+N32</f>
+        <v>19760</v>
+      </c>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C33" s="3">
         <v>6</v>
       </c>
@@ -1308,7 +1436,7 @@
       <c r="F33" s="7">
         <v>8868</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <f t="shared" si="5"/>
         <v>19760</v>
       </c>
@@ -1328,8 +1456,24 @@
         <f>K33+J33+I33</f>
         <v>19760</v>
       </c>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M33" s="3">
+        <v>6</v>
+      </c>
+      <c r="N33" s="7">
+        <v>4911</v>
+      </c>
+      <c r="O33" s="7">
+        <v>9891</v>
+      </c>
+      <c r="P33" s="7">
+        <v>4958</v>
+      </c>
+      <c r="Q33" s="1">
+        <f>P33+O33+N33</f>
+        <v>19760</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C34" s="3">
         <v>7</v>
       </c>
@@ -1340,11 +1484,11 @@
         <v>5544</v>
       </c>
       <c r="F34" s="7">
-        <v>5544</v>
-      </c>
-      <c r="G34">
+        <v>7828</v>
+      </c>
+      <c r="G34" s="1">
         <f t="shared" si="5"/>
-        <v>17476</v>
+        <v>19760</v>
       </c>
       <c r="H34" s="3">
         <v>7</v>
@@ -1362,8 +1506,24 @@
         <f>K34+J34+I34</f>
         <v>19760</v>
       </c>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M34" s="3">
+        <v>7</v>
+      </c>
+      <c r="N34" s="7">
+        <v>4787</v>
+      </c>
+      <c r="O34" s="7">
+        <v>9442</v>
+      </c>
+      <c r="P34" s="7">
+        <v>5531</v>
+      </c>
+      <c r="Q34" s="1">
+        <f>P34+O34+N34</f>
+        <v>19760</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C35" s="3">
         <v>8</v>
       </c>
@@ -1376,7 +1536,7 @@
       <c r="F35" s="7">
         <v>10663</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <f t="shared" si="5"/>
         <v>19760</v>
       </c>
@@ -1394,6 +1554,22 @@
       </c>
       <c r="L35" s="1">
         <f>K35+J35+I35</f>
+        <v>19760</v>
+      </c>
+      <c r="M35" s="3">
+        <v>8</v>
+      </c>
+      <c r="N35" s="7">
+        <v>5137</v>
+      </c>
+      <c r="O35" s="7">
+        <v>10459</v>
+      </c>
+      <c r="P35" s="7">
+        <v>4164</v>
+      </c>
+      <c r="Q35" s="1">
+        <f>P35+O35+N35</f>
         <v>19760</v>
       </c>
     </row>

</xml_diff>